<commit_message>
增加 LocationComponent 组件 未完成
</commit_message>
<xml_diff>
--- a/conf_xlsx/Config_StartConfig.xlsx
+++ b/conf_xlsx/Config_StartConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Mu\ProjectGameServer\MiracleServer\etc_server\conf_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEFF3CD-8101-4C5C-92C9-AC5A9C32BE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F289585C-B36D-4A93-91C3-3D90F5C2A423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="285" windowWidth="25320" windowHeight="13395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1890" yWindow="2805" windowWidth="25320" windowHeight="13395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -88,10 +88,6 @@
   </si>
   <si>
     <t>127.0.0.1:10025</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>127.0.0.1:10001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -453,7 +449,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -464,7 +460,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -512,10 +508,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -526,10 +522,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -543,7 +539,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -554,7 +550,7 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -565,7 +561,7 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -576,7 +572,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -587,7 +583,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>